<commit_message>
New certificate about C Programming added
</commit_message>
<xml_diff>
--- a/certificates/certifications-list.xlsx
+++ b/certificates/certifications-list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BBE999-8F20-4283-8769-F588CE2CDC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE95E03-66D8-42A4-BFF8-B561C80D1C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>COURSE NAME</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/certificate/UC-acb11d70-fc58-4488-b4a8-3b5161b07040/</t>
   </si>
 </sst>
 </file>
@@ -540,54 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,6 +565,54 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -895,7 +898,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,10 +911,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="40"/>
       <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
@@ -923,10 +926,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -940,8 +943,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="43"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -953,8 +956,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="43"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
@@ -966,17 +969,19 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="23" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="24"/>
+      <c r="D5" s="8">
+        <v>44380</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
@@ -986,10 +991,10 @@
       <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="33"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1008,10 +1013,10 @@
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1025,8 +1030,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
@@ -1038,8 +1043,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="40"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="13" t="s">
         <v>22</v>
       </c>
@@ -1051,8 +1056,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="13" t="s">
         <v>25</v>
       </c>
@@ -1064,8 +1069,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="13" t="s">
         <v>28</v>
       </c>
@@ -1077,8 +1082,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="40"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="13" t="s">
         <v>31</v>
       </c>
@@ -1090,8 +1095,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
-      <c r="B15" s="40"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
@@ -1103,8 +1108,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="16" t="s">
         <v>37</v>
       </c>
@@ -1145,29 +1150,29 @@
       <c r="C19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="36" t="s">
         <v>54</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="47"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="53">
+      <c r="D21" s="37">
         <v>44377</v>
       </c>
       <c r="E21" s="24" t="s">
@@ -1182,14 +1187,14 @@
       <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="30"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="52" t="s">
+      <c r="D23" s="36" t="s">
         <v>54</v>
       </c>
       <c r="E23" s="6"/>
@@ -1226,8 +1231,9 @@
     <hyperlink ref="E16" r:id="rId12" xr:uid="{571F4791-607B-4361-9380-35B9E3FA4450}"/>
     <hyperlink ref="E17" r:id="rId13" xr:uid="{1FF886F6-B677-4AA2-9416-4F63D80219C9}"/>
     <hyperlink ref="E21" r:id="rId14" xr:uid="{ADB7B64C-849C-4D38-AC6A-88FF599384B9}"/>
+    <hyperlink ref="E5" r:id="rId15" xr:uid="{682A56EC-7DE8-43A8-8AF6-20F43650707D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>